<commit_message>
[OP] Actualización de los documentos, planes, estados, riesgos
</commit_message>
<xml_diff>
--- a/_Control del Proyecto/Planilla de Trabajo HH.xlsx
+++ b/_Control del Proyecto/Planilla de Trabajo HH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanka\Dropbox\Proyecto OPServices\_Control del Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pizarro Spreng\Dropbox\Proyecto OPServices\_Control del Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t xml:space="preserve">Fecha </t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Pagina Express</t>
+  </si>
+  <si>
+    <t>Control de Proyecto</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,7 +532,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -540,7 +542,6 @@
     <xf numFmtId="20" fontId="4" fillId="5" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Énfasis1" xfId="5" builtinId="32"/>
@@ -830,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,21 +848,22 @@
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
-      <c r="G1" s="32" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
@@ -952,8 +954,8 @@
         <v>44</v>
       </c>
       <c r="S3" s="26">
-        <f>(194)*S2</f>
-        <v>955644</v>
+        <f>(217.38)*S2</f>
+        <v>1070813.8799999999</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
@@ -1060,6 +1062,10 @@
       <c r="O6" s="8">
         <f t="shared" si="1"/>
         <v>0.16527777777777775</v>
+      </c>
+      <c r="Q6" s="11">
+        <f xml:space="preserve"> Q8+R8</f>
+        <v>9.0680555555555546</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -1135,6 +1141,12 @@
         <f t="shared" si="1"/>
         <v>4.4444444444444398E-2</v>
       </c>
+      <c r="Q8" s="11">
+        <v>8.0416666666666661</v>
+      </c>
+      <c r="R8" s="11">
+        <v>1.0263888888888888</v>
+      </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="18">
@@ -1641,51 +1653,126 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="35">
-        <v>41563</v>
-      </c>
-      <c r="C25" s="29">
-        <v>0.75138888888888899</v>
-      </c>
-      <c r="G25" s="35">
-        <v>41563</v>
-      </c>
-      <c r="H25" s="29">
-        <v>0.75138888888888899</v>
-      </c>
-      <c r="I25" s="29"/>
+      <c r="B25" s="18">
+        <v>41570</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="18">
+        <v>41570</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H26" s="29"/>
+      <c r="B26" s="18">
+        <v>41570</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="18">
+        <v>41570</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="H27" s="29"/>
+      <c r="B27" s="18">
+        <v>41570</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="18">
+        <v>41570</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="I27" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="29"/>
-      <c r="H28" s="31"/>
+      <c r="B28" s="18">
+        <v>41570</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29">
+        <v>0.16041666666666668</v>
+      </c>
       <c r="H29" s="29"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="11">
-        <f>45+149</f>
-        <v>194</v>
-      </c>
-      <c r="G30">
-        <f>149+45</f>
-        <v>194</v>
-      </c>
+      <c r="C30" s="11">
+        <f>D31+E31</f>
+        <v>1.026388888888889</v>
+      </c>
+      <c r="D30" s="29">
+        <v>0.12430555555555556</v>
+      </c>
+      <c r="E30" s="11"/>
       <c r="H30" s="29"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="29"/>
+      <c r="C31" s="29">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="D31" s="29">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="E31" s="29">
+        <v>0.55625000000000002</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1702,7 +1789,7 @@
   <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,12 +1824,12 @@
         <v>41</v>
       </c>
       <c r="C3" s="25">
-        <f>SUM(C9:C10)+103446</f>
-        <v>1879886</v>
+        <f>SUM(C9:C10)+133446</f>
+        <v>2025055.88</v>
       </c>
       <c r="D3" s="28">
         <f>C3*D2/C2</f>
-        <v>32.283212381294042</v>
+        <v>34.776209332921411</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1751,11 +1838,11 @@
       </c>
       <c r="C4" s="26">
         <f>C2-C3</f>
-        <v>3943221</v>
+        <v>3798051.12</v>
       </c>
       <c r="D4" s="28">
         <f>C4*D2/C2</f>
-        <v>67.716787618705965</v>
+        <v>65.223790667078589</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -1772,7 +1859,7 @@
       </c>
       <c r="C10" s="26">
         <f>HH!S3</f>
-        <v>955644</v>
+        <v>1070813.8799999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[OP] [OP] Nuevo orden en los documentos, actualizacion de docuemntos.
</commit_message>
<xml_diff>
--- a/_Control del Proyecto/Planilla de Trabajo HH.xlsx
+++ b/_Control del Proyecto/Planilla de Trabajo HH.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pizarro Spreng\Dropbox\Proyecto OPServices\_Control del Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos de Programa\Dropbox\Proyecto OPServices\_Control del Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HH" sheetId="1" r:id="rId1"/>
@@ -832,26 +832,26 @@
   <dimension ref="B1:S31"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="31" t="s">
         <v>34</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="33"/>
     </row>
-    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
@@ -909,7 +909,7 @@
         <v>4926</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="18">
         <v>41507</v>
       </c>
@@ -954,11 +954,11 @@
         <v>44</v>
       </c>
       <c r="S3" s="26">
-        <f>(217.38)*S2</f>
-        <v>1070813.8799999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+        <f>(284.03)*S2</f>
+        <v>1399131.7799999998</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>41507</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0.32777777777777783</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>41508</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>41512</v>
       </c>
@@ -1064,11 +1064,11 @@
         <v>0.16527777777777775</v>
       </c>
       <c r="Q6" s="11">
-        <f xml:space="preserve"> Q8+R8</f>
-        <v>9.0680555555555546</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+        <f xml:space="preserve"> Q8+R8+R9+R10+R11</f>
+        <v>11.835416666666665</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="18">
         <v>41513</v>
       </c>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="P7" s="9"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>41513</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>1.0263888888888888</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>41513</v>
       </c>
@@ -1182,8 +1182,11 @@
         <f t="shared" si="1"/>
         <v>0.1694444444444444</v>
       </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R9" s="11">
+        <v>0.98472222222222217</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>41514</v>
       </c>
@@ -1216,8 +1219,11 @@
         <f t="shared" si="1"/>
         <v>5.1388888888888928E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R10" s="11">
+        <v>0.84305555555555556</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
         <v>41520</v>
       </c>
@@ -1249,8 +1255,11 @@
         <f t="shared" si="1"/>
         <v>0.2416666666666667</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="R11" s="11">
+        <v>0.93958333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
         <v>41521</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
         <v>41521</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>9.9305555555555536E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
         <v>41523</v>
       </c>
@@ -1351,7 +1360,7 @@
         <v>0.14722222222222237</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="18">
         <v>41523</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>0.38055555555555554</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="18">
         <v>41527</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>0.29583333333333339</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="18">
         <v>41528</v>
       </c>
@@ -1452,7 +1461,7 @@
         <v>0.10625</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="18">
         <v>41528</v>
       </c>
@@ -1484,7 +1493,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="18">
         <v>41548</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>6.3888888888888884E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="18">
         <v>41553</v>
       </c>
@@ -1547,8 +1556,9 @@
       <c r="O20" s="8">
         <v>0.26111111111111113</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R20" s="29"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="18">
         <v>41553</v>
       </c>
@@ -1574,7 +1584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="18">
         <v>41555</v>
       </c>
@@ -1600,7 +1610,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="18">
         <v>41556</v>
       </c>
@@ -1626,7 +1636,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="18">
         <v>41556</v>
       </c>
@@ -1652,7 +1662,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B25" s="18">
         <v>41570</v>
       </c>
@@ -1678,7 +1688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="18">
         <v>41570</v>
       </c>
@@ -1704,7 +1714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="18">
         <v>41570</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="18">
         <v>41570</v>
       </c>
@@ -1745,14 +1755,14 @@
       </c>
       <c r="H28" s="30"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C29" s="29"/>
       <c r="D29" s="29">
         <v>0.16041666666666668</v>
       </c>
       <c r="H29" s="29"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C30" s="11">
         <f>D31+E31</f>
         <v>1.026388888888889</v>
@@ -1763,7 +1773,7 @@
       <c r="E30" s="11"/>
       <c r="H30" s="29"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C31" s="29">
         <v>0.18541666666666667</v>
       </c>
@@ -1789,17 +1799,17 @@
   <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>39</v>
       </c>
@@ -1807,7 +1817,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>38</v>
       </c>
@@ -1819,33 +1829,33 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="25">
         <f>SUM(C9:C10)+133446</f>
-        <v>2025055.88</v>
+        <v>2353373.7799999998</v>
       </c>
       <c r="D3" s="28">
         <f>C3*D2/C2</f>
-        <v>34.776209332921411</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <v>40.414400422317499</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="26">
         <f>C2-C3</f>
-        <v>3798051.12</v>
+        <v>3469733.22</v>
       </c>
       <c r="D4" s="28">
         <f>C4*D2/C2</f>
-        <v>65.223790667078589</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>59.585599577682501</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1853,13 +1863,13 @@
         <v>820796</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="26">
         <f>HH!S3</f>
-        <v>1070813.8799999999</v>
+        <v>1399131.7799999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de Documentos y aplicación para hito 3
</commit_message>
<xml_diff>
--- a/_Control del Proyecto/Planilla de Trabajo HH.xlsx
+++ b/_Control del Proyecto/Planilla de Trabajo HH.xlsx
@@ -473,7 +473,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,6 +542,7 @@
     <xf numFmtId="20" fontId="4" fillId="5" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="60% - Énfasis1" xfId="5" builtinId="32"/>
@@ -832,7 +833,7 @@
   <dimension ref="B1:S31"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,6 +848,7 @@
     <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -954,8 +956,8 @@
         <v>44</v>
       </c>
       <c r="S3" s="26">
-        <f>(284.03)*S2</f>
-        <v>1399131.7799999998</v>
+        <f>(314.25)*S2</f>
+        <v>1547995.5</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
@@ -1064,8 +1066,8 @@
         <v>0.16527777777777775</v>
       </c>
       <c r="Q6" s="11">
-        <f xml:space="preserve"> Q8+R8+R9+R10+R11</f>
-        <v>11.835416666666665</v>
+        <f xml:space="preserve"> Q8+R8+R9+R10+R11+R12</f>
+        <v>13.100694444444443</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="18" customHeight="1" x14ac:dyDescent="0.5">
@@ -1141,7 +1143,7 @@
         <f t="shared" si="1"/>
         <v>4.4444444444444398E-2</v>
       </c>
-      <c r="Q8" s="11">
+      <c r="Q8" s="34">
         <v>8.0416666666666661</v>
       </c>
       <c r="R8" s="11">
@@ -1290,6 +1292,9 @@
       </c>
       <c r="O12" s="8">
         <v>0.1875</v>
+      </c>
+      <c r="R12" s="11">
+        <v>1.2652777777777777</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
@@ -1799,7 +1804,7 @@
   <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1835,11 +1840,11 @@
       </c>
       <c r="C3" s="25">
         <f>SUM(C9:C10)+133446</f>
-        <v>2353373.7799999998</v>
+        <v>2502237.5</v>
       </c>
       <c r="D3" s="28">
         <f>C3*D2/C2</f>
-        <v>40.414400422317499</v>
+        <v>42.970831550922902</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -1848,11 +1853,11 @@
       </c>
       <c r="C4" s="26">
         <f>C2-C3</f>
-        <v>3469733.22</v>
+        <v>3320869.5</v>
       </c>
       <c r="D4" s="28">
         <f>C4*D2/C2</f>
-        <v>59.585599577682501</v>
+        <v>57.029168449077098</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
@@ -1869,7 +1874,7 @@
       </c>
       <c r="C10" s="26">
         <f>HH!S3</f>
-        <v>1399131.7799999998</v>
+        <v>1547995.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>